<commit_message>
updating document and adding a test case
</commit_message>
<xml_diff>
--- a/Test Cases/ClassificationTestCases.xlsx
+++ b/Test Cases/ClassificationTestCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
   <si>
     <t>Testing for actual values taken from the dataset</t>
   </si>
@@ -79,6 +79,33 @@
   </si>
   <si>
     <t>current loan del sts output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max length </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Current UPB</t>
+  </si>
+  <si>
+    <t>Loan Age maxlength</t>
+  </si>
+  <si>
+    <t>Months to Legal Maturity</t>
+  </si>
+  <si>
+    <t>Current Interest Rate</t>
+  </si>
+  <si>
+    <t>Current Deferred UPB</t>
+  </si>
+  <si>
+    <t>Testing for  Max Length</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>UI doesn't allow User to enter</t>
   </si>
 </sst>
 </file>
@@ -574,10 +601,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -936,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,14 +990,14 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -990,18 +1018,18 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="3"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G3" t="s">
@@ -1575,6 +1603,74 @@
       </c>
       <c r="F27" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>